<commit_message>
added few more examples
</commit_message>
<xml_diff>
--- a/Flights_SearchResults_DataScraping.xlsx
+++ b/Flights_SearchResults_DataScraping.xlsx
@@ -4,7 +4,7 @@
   <x:fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <x:workbookPr codeName="ThisWorkbook"/>
   <x:bookViews>
-    <x:workbookView windowWidth="18650" windowHeight="7110" firstSheet="0" activeTab="2"/>
+    <x:workbookView windowWidth="18650" windowHeight="7110" firstSheet="0" activeTab="1"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <x:si>
     <x:t>FlightName</x:t>
   </x:si>
@@ -40,79 +40,103 @@
     <x:t>ArrivalTime</x:t>
   </x:si>
   <x:si>
+    <x:t>AirAsia India</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hyderabad, India</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Chennai, India</x:t>
+  </x:si>
+  <x:si>
+    <x:t>07:25</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0h 55m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3,135</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:20</x:t>
+  </x:si>
+  <x:si>
     <x:t>IndiGo</x:t>
   </x:si>
   <x:si>
-    <x:t>Hyderabad, India</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Chennai, India</x:t>
-  </x:si>
-  <x:si>
-    <x:t>18:45</x:t>
+    <x:t>06:20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1h 10m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>07:30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>18:00</x:t>
   </x:si>
   <x:si>
     <x:t>1h 25m</x:t>
   </x:si>
   <x:si>
-    <x:t>4,551</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20:10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Spicejet</x:t>
-  </x:si>
-  <x:si>
-    <x:t>18:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>14h 45m</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5,109</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:45</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Vistara</x:t>
-  </x:si>
-  <x:si>
-    <x:t>18:35</x:t>
-  </x:si>
-  <x:si>
-    <x:t>18h 00m</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9,003</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12:35</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Air India</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20:15</x:t>
-  </x:si>
-  <x:si>
-    <x:t>23h 25m</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9,769</x:t>
-  </x:si>
-  <x:si>
-    <x:t>19:40</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12:45</x:t>
-  </x:si>
-  <x:si>
-    <x:t>23h 50m</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11,838</x:t>
+    <x:t>3,449</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19:25</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TruJet</x:t>
+  </x:si>
+  <x:si>
+    <x:t>09:20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7h 10m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3,644</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16:30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TruJet, IndiGo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7h 20m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4,986</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15:40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8h 35m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16:55</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11h 05m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7h 00m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5,629</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8h 15m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>07:20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8h 20m</x:t>
   </x:si>
   <x:si>
     <x:t>Base Fare</x:t>
@@ -128,12 +152,6 @@
   </x:si>
   <x:si>
     <x:t>Add Ons</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Convenience Fee</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ticket Price</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -156,20 +174,6 @@
     </x:font>
     <x:font>
       <x:sz val="11"/>
-      <x:color theme="0"/>
-      <x:name val="Calibri"/>
-      <x:charset val="0"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:sz val="11"/>
-      <x:color theme="1"/>
-      <x:name val="Calibri"/>
-      <x:charset val="0"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:sz val="11"/>
       <x:color rgb="FFFF0000"/>
       <x:name val="Calibri"/>
       <x:charset val="0"/>
@@ -186,45 +190,39 @@
     <x:font>
       <x:b/>
       <x:sz val="11"/>
-      <x:color rgb="FFFFFFFF"/>
+      <x:color theme="3"/>
+      <x:name val="Calibri"/>
+      <x:charset val="134"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:sz val="18"/>
+      <x:color theme="3"/>
+      <x:name val="Calibri"/>
+      <x:charset val="134"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:u/>
+      <x:sz val="11"/>
+      <x:color rgb="FF0000FF"/>
       <x:name val="Calibri"/>
       <x:charset val="0"/>
       <x:scheme val="minor"/>
     </x:font>
     <x:font>
-      <x:sz val="11"/>
-      <x:color rgb="FF9C6500"/>
+      <x:i/>
+      <x:sz val="11"/>
+      <x:color rgb="FF7F7F7F"/>
       <x:name val="Calibri"/>
       <x:charset val="0"/>
       <x:scheme val="minor"/>
     </x:font>
     <x:font>
-      <x:b/>
-      <x:sz val="11"/>
-      <x:color theme="1"/>
-      <x:name val="Calibri"/>
-      <x:charset val="0"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:b/>
-      <x:sz val="11"/>
-      <x:color rgb="FF3F3F3F"/>
-      <x:name val="Calibri"/>
-      <x:charset val="0"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:b/>
-      <x:sz val="11"/>
-      <x:color rgb="FFFA7D00"/>
-      <x:name val="Calibri"/>
-      <x:charset val="0"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:sz val="11"/>
-      <x:color rgb="FFFA7D00"/>
+      <x:u/>
+      <x:sz val="11"/>
+      <x:color rgb="FF800080"/>
       <x:name val="Calibri"/>
       <x:charset val="0"/>
       <x:scheme val="minor"/>
@@ -239,6 +237,28 @@
     </x:font>
     <x:font>
       <x:sz val="11"/>
+      <x:color theme="0"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:sz val="11"/>
+      <x:color rgb="FFFFFFFF"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:sz val="11"/>
       <x:color rgb="FF9C0006"/>
       <x:name val="Calibri"/>
       <x:charset val="0"/>
@@ -246,6 +266,20 @@
     </x:font>
     <x:font>
       <x:sz val="11"/>
+      <x:color rgb="FFFA7D00"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:sz val="11"/>
+      <x:color rgb="FF3F3F76"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:sz val="11"/>
       <x:color rgb="FF006100"/>
       <x:name val="Calibri"/>
       <x:charset val="0"/>
@@ -254,46 +288,30 @@
     <x:font>
       <x:b/>
       <x:sz val="11"/>
-      <x:color theme="3"/>
-      <x:name val="Calibri"/>
-      <x:charset val="134"/>
+      <x:color rgb="FF3F3F3F"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:sz val="11"/>
+      <x:color rgb="FF9C6500"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
       <x:scheme val="minor"/>
     </x:font>
     <x:font>
       <x:b/>
-      <x:sz val="18"/>
-      <x:color theme="3"/>
-      <x:name val="Calibri"/>
-      <x:charset val="134"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:u/>
-      <x:sz val="11"/>
-      <x:color rgb="FF0000FF"/>
+      <x:sz val="11"/>
+      <x:color rgb="FFFA7D00"/>
       <x:name val="Calibri"/>
       <x:charset val="0"/>
       <x:scheme val="minor"/>
     </x:font>
     <x:font>
-      <x:sz val="11"/>
-      <x:color rgb="FF3F3F76"/>
-      <x:name val="Calibri"/>
-      <x:charset val="0"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:i/>
-      <x:sz val="11"/>
-      <x:color rgb="FF7F7F7F"/>
-      <x:name val="Calibri"/>
-      <x:charset val="0"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:u/>
-      <x:sz val="11"/>
-      <x:color rgb="FF800080"/>
+      <x:b/>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
       <x:name val="Calibri"/>
       <x:charset val="0"/>
       <x:scheme val="minor"/>
@@ -315,31 +333,145 @@
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFFFFFCC"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="4" tint="0.399975585192419"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="6" tint="0.399975585192419"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFA5A5A5"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="9" tint="0.599993896298105"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="8" tint="0.599993896298105"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFFFC7CE"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="4" tint="0.599993896298105"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="8"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="6" tint="0.599993896298105"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="7" tint="0.399975585192419"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="7"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="4"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFFFCC99"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="5" tint="0.599993896298105"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="7" tint="0.599993896298105"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="5" tint="0.799981688894314"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="8" tint="0.799981688894314"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="4" tint="0.799981688894314"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFC6EFCE"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="8" tint="0.399975585192419"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="6"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
         <x:fgColor theme="5" tint="0.399975585192419"/>
         <x:bgColor indexed="64"/>
       </x:patternFill>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
-        <x:fgColor theme="5" tint="0.799981688894314"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor theme="4"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor theme="4" tint="0.799981688894314"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor theme="6" tint="0.399975585192419"/>
+        <x:fgColor rgb="FFF2F2F2"/>
         <x:bgColor indexed="64"/>
       </x:patternFill>
     </x:fill>
@@ -351,25 +483,13 @@
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
-        <x:fgColor theme="7" tint="0.399975585192419"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor rgb="FFA5A5A5"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor theme="6"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor theme="8" tint="0.799981688894314"/>
+        <x:fgColor theme="6" tint="0.799981688894314"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="9" tint="0.799981688894314"/>
         <x:bgColor indexed="64"/>
       </x:patternFill>
     </x:fill>
@@ -381,121 +501,19 @@
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
+        <x:fgColor theme="9"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
         <x:fgColor theme="7" tint="0.799981688894314"/>
         <x:bgColor indexed="64"/>
       </x:patternFill>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
-        <x:fgColor theme="7"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor rgb="FFF2F2F2"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor theme="5" tint="0.599993896298105"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor theme="4" tint="0.599993896298105"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor theme="9"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor theme="8" tint="0.399975585192419"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor theme="6" tint="0.599993896298105"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor theme="8"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
         <x:fgColor theme="5"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor rgb="FFFFFFCC"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor theme="8" tint="0.599993896298105"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor theme="7" tint="0.599993896298105"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor theme="6" tint="0.799981688894314"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor rgb="FFFFC7CE"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor rgb="FFC6EFCE"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor theme="9" tint="0.599993896298105"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor theme="9" tint="0.799981688894314"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor theme="4" tint="0.399975585192419"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor rgb="FFFFCC99"/>
         <x:bgColor indexed="64"/>
       </x:patternFill>
     </x:fill>
@@ -514,6 +532,30 @@
       <x:top/>
       <x:bottom style="medium">
         <x:color theme="4"/>
+      </x:bottom>
+      <x:diagonal/>
+    </x:border>
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom style="medium">
+        <x:color theme="4" tint="0.499984740745262"/>
+      </x:bottom>
+      <x:diagonal/>
+    </x:border>
+    <x:border>
+      <x:left style="thin">
+        <x:color rgb="FFB2B2B2"/>
+      </x:left>
+      <x:right style="thin">
+        <x:color rgb="FFB2B2B2"/>
+      </x:right>
+      <x:top style="thin">
+        <x:color rgb="FFB2B2B2"/>
+      </x:top>
+      <x:bottom style="thin">
+        <x:color rgb="FFB2B2B2"/>
       </x:bottom>
       <x:diagonal/>
     </x:border>
@@ -535,11 +577,24 @@
     <x:border>
       <x:left/>
       <x:right/>
+      <x:top/>
+      <x:bottom style="double">
+        <x:color rgb="FFFF8001"/>
+      </x:bottom>
+      <x:diagonal/>
+    </x:border>
+    <x:border>
+      <x:left style="thin">
+        <x:color rgb="FF7F7F7F"/>
+      </x:left>
+      <x:right style="thin">
+        <x:color rgb="FF7F7F7F"/>
+      </x:right>
       <x:top style="thin">
-        <x:color theme="4"/>
+        <x:color rgb="FF7F7F7F"/>
       </x:top>
-      <x:bottom style="double">
-        <x:color theme="4"/>
+      <x:bottom style="thin">
+        <x:color rgb="FF7F7F7F"/>
       </x:bottom>
       <x:diagonal/>
     </x:border>
@@ -559,57 +614,20 @@
       <x:diagonal/>
     </x:border>
     <x:border>
-      <x:left style="thin">
-        <x:color rgb="FF7F7F7F"/>
-      </x:left>
-      <x:right style="thin">
-        <x:color rgb="FF7F7F7F"/>
-      </x:right>
-      <x:top style="thin">
-        <x:color rgb="FF7F7F7F"/>
-      </x:top>
-      <x:bottom style="thin">
-        <x:color rgb="FF7F7F7F"/>
-      </x:bottom>
-      <x:diagonal/>
-    </x:border>
-    <x:border>
       <x:left/>
       <x:right/>
-      <x:top/>
+      <x:top style="thin">
+        <x:color theme="4"/>
+      </x:top>
       <x:bottom style="double">
-        <x:color rgb="FFFF8001"/>
-      </x:bottom>
-      <x:diagonal/>
-    </x:border>
-    <x:border>
-      <x:left style="thin">
-        <x:color rgb="FFB2B2B2"/>
-      </x:left>
-      <x:right style="thin">
-        <x:color rgb="FFB2B2B2"/>
-      </x:right>
-      <x:top style="thin">
-        <x:color rgb="FFB2B2B2"/>
-      </x:top>
-      <x:bottom style="thin">
-        <x:color rgb="FFB2B2B2"/>
-      </x:bottom>
-      <x:diagonal/>
-    </x:border>
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom style="medium">
-        <x:color theme="4" tint="0.499984740745262"/>
+        <x:color theme="4"/>
       </x:bottom>
       <x:diagonal/>
     </x:border>
   </x:borders>
   <x:cellStyleXfs count="50">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <x:xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <x:xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <x:alignment vertical="center"/>
     </x:xf>
     <x:xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -627,130 +645,130 @@
     <x:xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <x:alignment vertical="center"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="5" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <x:xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <x:alignment vertical="center"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <x:alignment vertical="center"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="17" fillId="32" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="8" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="9" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <x:alignment vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <x:xf numFmtId="0" fontId="14" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="16" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="18" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <x:alignment vertical="center"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -1085,13 +1103,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:G6"/>
+  <x:dimension ref="A1:G11"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
-      <x:selection activeCell="A2" sqref="A2 A2:A2"/>
+      <x:selection activeCell="B6" sqref="B6 B6:B6"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="44.968352" defaultRowHeight="14.5"/>
+  <x:sheetFormatPr defaultColWidth="56.334943" defaultRowHeight="14.5"/>
   <x:sheetData>
     <x:row r="1" spans="1:7">
       <x:c r="A1" s="2" t="s">
@@ -1156,15 +1174,15 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F3" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="G3" s="2" t="s">
         <x:v>17</x:v>
-      </x:c>
-      <x:c r="G3" s="2" t="s">
-        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:7">
       <x:c r="A4" s="2" t="s">
-        <x:v>19</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B4" s="2" t="s">
         <x:v>8</x:v>
@@ -1173,21 +1191,21 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D4" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E4" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="F4" s="2" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="E4" s="2" t="s">
+      <x:c r="G4" s="2" t="s">
         <x:v>21</x:v>
-      </x:c>
-      <x:c r="F4" s="2" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="G4" s="2" t="s">
-        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:7">
       <x:c r="A5" s="2" t="s">
-        <x:v>24</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B5" s="2" t="s">
         <x:v>8</x:v>
@@ -1196,21 +1214,21 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D5" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E5" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F5" s="2" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="E5" s="2" t="s">
+      <x:c r="G5" s="2" t="s">
         <x:v>26</x:v>
-      </x:c>
-      <x:c r="F5" s="2" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="G5" s="2" t="s">
-        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:7">
       <x:c r="A6" s="2" t="s">
-        <x:v>19</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B6" s="2" t="s">
         <x:v>8</x:v>
@@ -1219,16 +1237,131 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D6" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E6" s="2" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="F6" s="2" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="E6" s="2" t="s">
+      <x:c r="G6" s="2" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="F6" s="2" t="s">
+    </x:row>
+    <x:row r="7" spans="1:7">
+      <x:c r="A7" s="2" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B7" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C7" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D7" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E7" s="2" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G6" s="2" t="s">
-        <x:v>23</x:v>
+      <x:c r="F7" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="G7" s="2" t="s">
+        <x:v>32</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:7">
+      <x:c r="A8" s="2" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B8" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C8" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D8" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E8" s="2" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="F8" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="G8" s="2" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:7">
+      <x:c r="A9" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B9" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C9" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D9" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="E9" s="2" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F9" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="G9" s="2" t="s">
+        <x:v>30</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:7">
+      <x:c r="A10" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B10" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C10" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D10" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="E10" s="2" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="F10" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="G10" s="2" t="s">
+        <x:v>32</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:7">
+      <x:c r="A11" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B11" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C11" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D11" s="2" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="E11" s="2" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="F11" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="G11" s="2" t="s">
+        <x:v>30</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1245,40 +1378,39 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B3"/>
+  <x:dimension ref="A1:B4"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0">
-      <x:selection activeCell="A4" sqref="A4 A4:A4"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="A15" sqref="A15 A15:A15"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="44.968352" defaultRowHeight="14.5"/>
+  <x:sheetFormatPr defaultColWidth="56.334943" defaultRowHeight="14.5"/>
   <x:sheetData>
     <x:row r="1" spans="1:2">
       <x:c r="A1" s="2" t="s">
-        <x:v>32</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B1" s="2" t="s">
-        <x:v>33</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:2">
       <x:c r="A2" s="2" t="s">
-        <x:v>34</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B2" s="2" t="s">
-        <x:v>35</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:2">
       <x:c r="A3" s="2" t="s">
-        <x:v>36</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:2">
-      <x:c r="A4" s="2" t="s">
-        <x:v>37</x:v>
-      </x:c>
-    </x:row>
+      <x:c r="A4" s="2" t="s"/>
+    </x:row>
+    <x:row r="15" spans="1:2"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1295,22 +1427,20 @@
   </x:sheetPr>
   <x:dimension ref="A1"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A2" sqref="A2 A2:A2"/>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="B12" sqref="B12 B12:B12"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="15.122898" defaultRowHeight="14.5"/>
+  <x:sheetFormatPr defaultColWidth="26.489489" defaultRowHeight="14.5"/>
   <x:sheetData>
-    <x:row r="1" spans="1:1">
-      <x:c r="A1" s="2" t="s">
-        <x:v>38</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:1"/>
+    <x:row r="1" spans="1:2">
+      <x:c r="A1" s="2" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:2"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>

</xml_diff>